<commit_message>
Changes inlcudes configuration of kalyana yatra email id and to fix the image rendering issue in the kalyanayatra email.
</commit_message>
<xml_diff>
--- a/src/main/resources/Kalyana Yatra Devotees - Master Sheet.xlsx
+++ b/src/main/resources/Kalyana Yatra Devotees - Master Sheet.xlsx
@@ -8,12 +8,13 @@
   </bookViews>
   <sheets>
     <sheet name="1008KY" sheetId="1" r:id="rId1"/>
-    <sheet name="108 -KYNMS Yet to be Completed" sheetId="2" r:id="rId2"/>
-    <sheet name="108DD" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet2" sheetId="5" r:id="rId2"/>
+    <sheet name="108 -KYNMS Yet to be Completed" sheetId="2" r:id="rId3"/>
+    <sheet name="108DD" sheetId="3" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="D1:P25"/>
+  <oleSize ref="D1:P24"/>
 </workbook>
 </file>
 
@@ -80,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1359" uniqueCount="721">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1346" uniqueCount="685">
   <si>
     <t xml:space="preserve">SitaRama Kalyanam Yatra
 </t>
@@ -2052,9 +2053,6 @@
     <t>Devotee Name</t>
   </si>
   <si>
-    <t>Cary</t>
-  </si>
-  <si>
     <t>harithasrinivas2013@gmail.com</t>
   </si>
   <si>
@@ -2115,24 +2113,6 @@
     <t>Smt.Swapna</t>
   </si>
   <si>
-    <t>Kaligotla</t>
-  </si>
-  <si>
-    <t>Srikar Prasad</t>
-  </si>
-  <si>
-    <t>Shathabhisha</t>
-  </si>
-  <si>
-    <t>Srimedha</t>
-  </si>
-  <si>
-    <t>Sriyansh</t>
-  </si>
-  <si>
-    <t>919-720-1359</t>
-  </si>
-  <si>
     <t>Sri.Srinivas</t>
   </si>
   <si>
@@ -2151,100 +2131,13 @@
     <t xml:space="preserve">919-443-8039(R) </t>
   </si>
   <si>
-    <t>Kayam</t>
-  </si>
-  <si>
-    <t>Pulipala</t>
-  </si>
-  <si>
-    <t>Sirish</t>
-  </si>
-  <si>
-    <t>312-420-5668</t>
-  </si>
-  <si>
-    <t>Gundlapudi</t>
-  </si>
-  <si>
-    <t>Bharadwajasa</t>
-  </si>
-  <si>
-    <t>Sailasya</t>
-  </si>
-  <si>
-    <t>Mohanasai Vamsi</t>
-  </si>
-  <si>
-    <t>Makha</t>
-  </si>
-  <si>
-    <t>Sri.Kishore</t>
-  </si>
-  <si>
-    <t>Smt.Suneetha</t>
-  </si>
-  <si>
     <t>Smt.Bindu Bhargavi</t>
   </si>
   <si>
-    <t xml:space="preserve">Sri.Sunil Kumar Reddy </t>
-  </si>
-  <si>
-    <t>Smt.Shireen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sri.Ravi </t>
-  </si>
-  <si>
-    <t>Smt.Madhavi</t>
-  </si>
-  <si>
-    <t>Glen Allen</t>
-  </si>
-  <si>
-    <t>804-396-8773</t>
-  </si>
-  <si>
-    <t>Vemulapalli</t>
-  </si>
-  <si>
-    <t>Pamidipala</t>
-  </si>
-  <si>
-    <t>Harshith</t>
-  </si>
-  <si>
-    <t>Chakri</t>
-  </si>
-  <si>
-    <t>919-986-5799</t>
-  </si>
-  <si>
-    <t>Sri.Prasad</t>
-  </si>
-  <si>
-    <t>Smt.Madhuri</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Balasubramanian </t>
-  </si>
-  <si>
-    <t>Haritha</t>
-  </si>
-  <si>
-    <t>Shyam</t>
-  </si>
-  <si>
-    <t>Sashwat</t>
-  </si>
-  <si>
-    <t>313-942-5169</t>
-  </si>
-  <si>
-    <t>Sri.Yegna</t>
-  </si>
-  <si>
-    <t>Smt.Kamakshi</t>
+    <t>swapnab29@gmail.com</t>
+  </si>
+  <si>
+    <t>boggarambb@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -2580,8 +2473,8 @@
     <xf numFmtId="164" fontId="11" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3513,6 +3406,222 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>714375</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="16" name="AutoShape 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9D3D8AF0-478F-4AE5-8B1A-CAB46DD91373}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>714375</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="17" name="AutoShape 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A45F0649-0C12-446D-93D7-4ABB4FA020BD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>714375</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="18" name="AutoShape 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CDA4A1C4-F632-4CE5-939E-C910AE797F5B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>714375</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="19" name="AutoShape 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1B776FD6-353B-4024-9DE7-89BF3BE22948}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -3815,7 +3924,7 @@
   <dimension ref="A1:P36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3895,13 +4004,13 @@
         <v>42657</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>683</v>
+        <v>676</v>
       </c>
       <c r="D2" s="24" t="s">
-        <v>684</v>
+        <v>677</v>
       </c>
       <c r="E2" s="25" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="F2" s="26"/>
       <c r="G2" s="27">
@@ -3917,7 +4026,7 @@
         <v>178</v>
       </c>
       <c r="K2" s="27" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="L2" s="28">
         <v>6025002960</v>
@@ -3926,14 +4035,14 @@
       <c r="N2" s="27"/>
       <c r="O2" s="27"/>
       <c r="P2" s="36" t="s">
-        <v>661</v>
+        <v>656</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="29"/>
       <c r="B3" s="30"/>
       <c r="C3" s="31" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="D3" s="32"/>
       <c r="E3" s="32" t="s">
@@ -3949,11 +4058,9 @@
       <c r="M3" s="28"/>
       <c r="N3" s="27"/>
       <c r="O3" s="27"/>
-      <c r="P3" s="36" t="s">
-        <v>657</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="P3" s="36"/>
+    </row>
+    <row r="4" spans="1:16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="22">
         <v>135</v>
       </c>
@@ -3961,13 +4068,13 @@
         <v>42658</v>
       </c>
       <c r="C4" s="24" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="D4" s="25" t="s">
+        <v>661</v>
+      </c>
+      <c r="E4" s="24" t="s">
         <v>662</v>
-      </c>
-      <c r="E4" s="24" t="s">
-        <v>663</v>
       </c>
       <c r="F4" s="26"/>
       <c r="G4" s="27">
@@ -3990,14 +4097,14 @@
       <c r="N4" s="27"/>
       <c r="O4" s="27"/>
       <c r="P4" s="36" t="s">
-        <v>661</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="29"/>
       <c r="B5" s="30"/>
       <c r="C5" s="31" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="D5" s="27"/>
       <c r="E5" s="32" t="s">
@@ -4015,11 +4122,11 @@
       <c r="O5" s="27"/>
       <c r="P5" s="36"/>
     </row>
-    <row r="6" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="29"/>
       <c r="B6" s="30"/>
       <c r="C6" s="31" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="D6" s="27"/>
       <c r="E6" s="32" t="s">
@@ -4037,15 +4144,15 @@
       <c r="O6" s="27"/>
       <c r="P6" s="36"/>
     </row>
-    <row r="7" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="29"/>
       <c r="B7" s="30"/>
       <c r="C7" s="31" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="D7" s="27"/>
       <c r="E7" s="32" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="F7" s="33"/>
       <c r="G7" s="27"/>
@@ -4059,7 +4166,7 @@
       <c r="O7" s="27"/>
       <c r="P7" s="36"/>
     </row>
-    <row r="8" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="38">
         <v>193</v>
       </c>
@@ -4067,36 +4174,36 @@
         <v>42910</v>
       </c>
       <c r="C8" s="25" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="D8" s="25" t="s">
+        <v>666</v>
+      </c>
+      <c r="E8" s="25" t="s">
         <v>667</v>
-      </c>
-      <c r="E8" s="25" t="s">
-        <v>668</v>
       </c>
       <c r="F8" s="25"/>
       <c r="J8" s="27" t="s">
         <v>151</v>
       </c>
       <c r="K8" s="27" t="s">
+        <v>670</v>
+      </c>
+      <c r="L8" s="28" t="s">
         <v>671</v>
-      </c>
-      <c r="L8" s="28" t="s">
-        <v>672</v>
       </c>
       <c r="M8" s="28"/>
       <c r="N8" s="28"/>
-      <c r="O8" s="28"/>
-      <c r="P8" s="28" t="s">
-        <v>661</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="O8" s="27"/>
+      <c r="P8" s="41" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="29"/>
       <c r="B9" s="30"/>
       <c r="C9" s="27" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="D9" s="27"/>
       <c r="E9" s="33" t="s">
@@ -4108,571 +4215,497 @@
       <c r="L9" s="28"/>
       <c r="M9" s="28"/>
       <c r="N9" s="28"/>
-      <c r="O9" s="28"/>
+      <c r="O9" s="27"/>
       <c r="P9" s="28"/>
     </row>
-    <row r="10" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="29"/>
       <c r="B10" s="30"/>
       <c r="C10" s="27" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="D10" s="27"/>
       <c r="E10" s="33" t="s">
         <v>36</v>
       </c>
       <c r="F10" s="33" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="J10" s="27"/>
       <c r="K10" s="27"/>
       <c r="L10" s="28"/>
       <c r="M10" s="28"/>
       <c r="N10" s="28"/>
-      <c r="O10" s="28"/>
+      <c r="O10" s="27"/>
       <c r="P10" s="28"/>
     </row>
-    <row r="11" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="38">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="B11" s="39">
-        <v>42988</v>
+        <v>42987</v>
       </c>
       <c r="C11" s="25" t="s">
-        <v>698</v>
+        <v>682</v>
       </c>
       <c r="D11" s="25" t="s">
-        <v>677</v>
+        <v>678</v>
       </c>
       <c r="E11" s="25" t="s">
-        <v>161</v>
+        <v>104</v>
       </c>
       <c r="F11" s="25" t="s">
-        <v>247</v>
+        <v>112</v>
       </c>
       <c r="J11" s="27" t="s">
         <v>178</v>
       </c>
       <c r="K11" s="27" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="L11" s="27" t="s">
-        <v>682</v>
-      </c>
-      <c r="M11" s="28"/>
+        <v>680</v>
+      </c>
+      <c r="M11" s="28" t="s">
+        <v>681</v>
+      </c>
       <c r="N11" s="28"/>
-      <c r="O11" s="28"/>
-      <c r="P11" s="28" t="s">
-        <v>661</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="O11" s="27"/>
+      <c r="P11" s="41" t="s">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="29"/>
       <c r="B12" s="40"/>
       <c r="C12" s="27" t="s">
-        <v>699</v>
+        <v>679</v>
       </c>
       <c r="D12" s="27"/>
       <c r="E12" s="33" t="s">
-        <v>20</v>
+        <v>156</v>
       </c>
       <c r="F12" s="33" t="s">
-        <v>177</v>
+        <v>37</v>
       </c>
       <c r="J12" s="27"/>
       <c r="K12" s="27"/>
       <c r="L12" s="27"/>
-      <c r="M12" s="28"/>
-      <c r="N12" s="28"/>
-      <c r="O12" s="28"/>
-      <c r="P12" s="28"/>
-    </row>
-    <row r="13" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="29"/>
-      <c r="B13" s="40"/>
-      <c r="C13" s="27" t="s">
-        <v>678</v>
-      </c>
-      <c r="D13" s="27"/>
-      <c r="E13" s="33" t="s">
-        <v>156</v>
-      </c>
-      <c r="F13" s="33" t="s">
-        <v>679</v>
-      </c>
-      <c r="J13" s="27"/>
-      <c r="K13" s="27"/>
-      <c r="L13" s="27"/>
-      <c r="M13" s="28"/>
-      <c r="N13" s="28"/>
-      <c r="O13" s="28"/>
-      <c r="P13" s="28"/>
-    </row>
-    <row r="14" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="29"/>
-      <c r="B14" s="40"/>
-      <c r="C14" s="27" t="s">
-        <v>680</v>
-      </c>
-      <c r="D14" s="27"/>
-      <c r="E14" s="33" t="s">
-        <v>666</v>
-      </c>
-      <c r="F14" s="33" t="s">
-        <v>21</v>
-      </c>
-      <c r="J14" s="27"/>
-      <c r="K14" s="27"/>
-      <c r="L14" s="27"/>
-      <c r="M14" s="28"/>
-      <c r="N14" s="28"/>
-      <c r="O14" s="28"/>
-      <c r="P14" s="28"/>
-    </row>
-    <row r="15" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="29"/>
-      <c r="B15" s="40"/>
-      <c r="C15" s="27" t="s">
-        <v>681</v>
-      </c>
-      <c r="D15" s="27"/>
-      <c r="E15" s="33" t="s">
-        <v>156</v>
-      </c>
-      <c r="F15" s="33" t="s">
-        <v>297</v>
-      </c>
-      <c r="J15" s="27"/>
-      <c r="K15" s="27"/>
-      <c r="L15" s="27"/>
-      <c r="M15" s="28"/>
-      <c r="N15" s="28"/>
-      <c r="O15" s="28"/>
-      <c r="P15" s="28"/>
-    </row>
-    <row r="16" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="38">
-        <v>238</v>
-      </c>
-      <c r="B16" s="39">
-        <v>42987</v>
-      </c>
-      <c r="C16" s="25" t="s">
-        <v>700</v>
-      </c>
-      <c r="D16" s="25" t="s">
-        <v>685</v>
-      </c>
-      <c r="E16" s="25" t="s">
-        <v>104</v>
-      </c>
-      <c r="F16" s="25" t="s">
-        <v>112</v>
-      </c>
-      <c r="J16" s="27" t="s">
-        <v>178</v>
-      </c>
-      <c r="K16" s="27" t="s">
-        <v>659</v>
-      </c>
-      <c r="L16" s="27" t="s">
-        <v>687</v>
-      </c>
-      <c r="M16" s="28" t="s">
-        <v>688</v>
-      </c>
-      <c r="N16" s="28"/>
-      <c r="O16" s="28"/>
-      <c r="P16" s="28" t="s">
-        <v>661</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="29"/>
-      <c r="B17" s="40"/>
-      <c r="C17" s="27" t="s">
-        <v>686</v>
-      </c>
-      <c r="D17" s="27"/>
-      <c r="E17" s="33" t="s">
-        <v>156</v>
-      </c>
-      <c r="F17" s="33" t="s">
-        <v>37</v>
-      </c>
-      <c r="J17" s="27"/>
-      <c r="K17" s="27"/>
-      <c r="L17" s="27"/>
-      <c r="M17" s="29"/>
-      <c r="N17" s="29"/>
-      <c r="O17" s="29"/>
-      <c r="P17" s="29"/>
-    </row>
-    <row r="18" spans="1:16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="38">
-        <v>94</v>
-      </c>
-      <c r="B18" s="39">
-        <v>42802</v>
-      </c>
-      <c r="C18" s="24" t="s">
-        <v>701</v>
-      </c>
-      <c r="D18" s="25" t="s">
-        <v>689</v>
-      </c>
-      <c r="E18" s="24" t="s">
-        <v>690</v>
-      </c>
-      <c r="F18" s="41"/>
-      <c r="J18" s="27" t="s">
-        <v>121</v>
-      </c>
-      <c r="K18" s="27" t="s">
-        <v>122</v>
-      </c>
-      <c r="L18" s="27" t="s">
-        <v>692</v>
-      </c>
-      <c r="M18" s="27"/>
-      <c r="N18" s="29"/>
-      <c r="O18" s="29"/>
-      <c r="P18" s="28" t="s">
-        <v>661</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="29"/>
-      <c r="B19" s="30"/>
-      <c r="C19" s="31" t="s">
-        <v>702</v>
-      </c>
-      <c r="D19" s="27"/>
-      <c r="E19" s="32" t="s">
-        <v>20</v>
-      </c>
-      <c r="F19" s="33"/>
-      <c r="J19" s="27"/>
-      <c r="K19" s="27"/>
-      <c r="L19" s="27"/>
-      <c r="M19" s="29"/>
-      <c r="N19" s="40"/>
-      <c r="O19" s="29"/>
-      <c r="P19" s="40"/>
-    </row>
-    <row r="20" spans="1:16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="29"/>
-      <c r="B20" s="30"/>
-      <c r="C20" s="31" t="s">
-        <v>691</v>
-      </c>
-      <c r="D20" s="27"/>
-      <c r="E20" s="32" t="s">
-        <v>36</v>
-      </c>
-      <c r="F20" s="33"/>
-      <c r="J20" s="27"/>
-      <c r="K20" s="27"/>
-      <c r="L20" s="27"/>
-      <c r="M20" s="29"/>
-      <c r="N20" s="40"/>
-      <c r="O20" s="29"/>
-      <c r="P20" s="40"/>
-    </row>
-    <row r="21" spans="1:16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="38">
-        <v>236</v>
-      </c>
-      <c r="B21" s="39">
-        <v>42960</v>
-      </c>
-      <c r="C21" s="25" t="s">
-        <v>703</v>
-      </c>
-      <c r="D21" s="25" t="s">
-        <v>693</v>
-      </c>
-      <c r="E21" s="25" t="s">
-        <v>694</v>
-      </c>
-      <c r="F21" s="25" t="s">
-        <v>83</v>
-      </c>
-      <c r="J21" s="27" t="s">
-        <v>151</v>
-      </c>
-      <c r="K21" s="27" t="s">
-        <v>705</v>
-      </c>
-      <c r="L21" s="27" t="s">
-        <v>706</v>
-      </c>
-      <c r="M21" s="27"/>
-      <c r="N21" s="27"/>
-      <c r="O21" s="27"/>
-      <c r="P21" s="28" t="s">
-        <v>661</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="29"/>
-      <c r="B22" s="40"/>
-      <c r="C22" s="27" t="s">
-        <v>704</v>
-      </c>
-      <c r="D22" s="27"/>
-      <c r="E22" s="33" t="s">
-        <v>20</v>
-      </c>
-      <c r="F22" s="33" t="s">
-        <v>670</v>
-      </c>
-      <c r="J22" s="27"/>
-      <c r="K22" s="27"/>
-      <c r="L22" s="27"/>
-      <c r="M22" s="27"/>
-      <c r="N22" s="27"/>
-      <c r="O22" s="27"/>
-      <c r="P22" s="27"/>
-    </row>
-    <row r="23" spans="1:16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="29"/>
-      <c r="B23" s="40"/>
-      <c r="C23" s="27" t="s">
-        <v>695</v>
-      </c>
-      <c r="D23" s="27"/>
-      <c r="E23" s="33" t="s">
-        <v>666</v>
-      </c>
-      <c r="F23" s="33" t="s">
-        <v>37</v>
-      </c>
-      <c r="J23" s="27"/>
-      <c r="K23" s="27"/>
-      <c r="L23" s="27"/>
-      <c r="M23" s="27"/>
-      <c r="N23" s="27"/>
-      <c r="O23" s="27"/>
-      <c r="P23" s="27"/>
-    </row>
-    <row r="24" spans="1:16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="29"/>
-      <c r="B24" s="40"/>
-      <c r="C24" s="27" t="s">
-        <v>696</v>
-      </c>
-      <c r="D24" s="27"/>
-      <c r="E24" s="33" t="s">
-        <v>156</v>
-      </c>
-      <c r="F24" s="33" t="s">
-        <v>697</v>
-      </c>
-      <c r="J24" s="27"/>
-      <c r="K24" s="27"/>
-      <c r="L24" s="27"/>
-      <c r="M24" s="27"/>
-      <c r="N24" s="27"/>
-      <c r="O24" s="27"/>
-      <c r="P24" s="27"/>
-    </row>
-    <row r="25" spans="1:16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="38">
-        <v>240</v>
-      </c>
-      <c r="B25" s="39">
-        <v>42987</v>
-      </c>
-      <c r="C25" s="25" t="s">
-        <v>712</v>
-      </c>
-      <c r="D25" s="25" t="s">
-        <v>707</v>
-      </c>
-      <c r="E25" s="25" t="s">
-        <v>708</v>
-      </c>
-      <c r="J25" s="27" t="s">
-        <v>178</v>
-      </c>
-      <c r="K25" s="27" t="s">
-        <v>656</v>
-      </c>
-      <c r="L25" s="27" t="s">
-        <v>711</v>
-      </c>
-      <c r="M25" s="27"/>
-      <c r="N25" s="27"/>
-      <c r="O25" s="27"/>
-      <c r="P25" s="28" t="s">
-        <v>661</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="29"/>
-      <c r="B26" s="40"/>
-      <c r="C26" s="27" t="s">
-        <v>713</v>
-      </c>
-      <c r="D26" s="27"/>
-      <c r="E26" s="33" t="s">
-        <v>20</v>
-      </c>
-      <c r="J26" s="27"/>
-      <c r="K26" s="27"/>
-      <c r="L26" s="27"/>
-      <c r="M26" s="27"/>
-      <c r="N26" s="27"/>
-      <c r="O26" s="27"/>
-      <c r="P26" s="27"/>
-    </row>
-    <row r="27" spans="1:16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="29"/>
-      <c r="B27" s="40"/>
-      <c r="C27" s="27" t="s">
-        <v>709</v>
-      </c>
-      <c r="D27" s="27"/>
-      <c r="E27" s="33" t="s">
-        <v>156</v>
-      </c>
-      <c r="J27" s="27"/>
-      <c r="K27" s="27"/>
-      <c r="L27" s="27"/>
-      <c r="M27" s="27"/>
-      <c r="N27" s="27"/>
-      <c r="O27" s="27"/>
-      <c r="P27" s="27"/>
-    </row>
-    <row r="28" spans="1:16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="29"/>
-      <c r="B28" s="40"/>
-      <c r="C28" s="27" t="s">
-        <v>710</v>
-      </c>
-      <c r="D28" s="27"/>
-      <c r="E28" s="33" t="s">
-        <v>156</v>
-      </c>
-      <c r="J28" s="27"/>
-      <c r="K28" s="27"/>
-      <c r="L28" s="27"/>
-      <c r="M28" s="27"/>
-      <c r="N28" s="27"/>
-      <c r="O28" s="27"/>
-      <c r="P28" s="27"/>
-    </row>
-    <row r="29" spans="1:16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="38">
-        <v>222</v>
-      </c>
-      <c r="B29" s="39">
-        <v>42923</v>
-      </c>
-      <c r="C29" s="25" t="s">
-        <v>719</v>
-      </c>
-      <c r="D29" s="25" t="s">
-        <v>714</v>
-      </c>
-      <c r="E29" s="25" t="s">
-        <v>715</v>
-      </c>
-      <c r="J29" s="27" t="s">
-        <v>163</v>
-      </c>
-      <c r="K29" s="27" t="s">
-        <v>173</v>
-      </c>
-      <c r="L29" s="27" t="s">
-        <v>718</v>
-      </c>
-      <c r="M29" s="27"/>
-      <c r="N29" s="27"/>
-      <c r="O29" s="27"/>
-      <c r="P29" s="28" t="s">
-        <v>661</v>
-      </c>
-    </row>
-    <row r="30" spans="1:16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="29"/>
-      <c r="B30" s="40"/>
-      <c r="C30" s="27" t="s">
-        <v>720</v>
-      </c>
-      <c r="D30" s="27"/>
-      <c r="E30" s="33" t="s">
-        <v>20</v>
-      </c>
-      <c r="J30" s="27"/>
-      <c r="K30" s="27"/>
-      <c r="L30" s="27"/>
-      <c r="M30" s="27"/>
-      <c r="N30" s="27"/>
-      <c r="O30" s="27"/>
-      <c r="P30" s="27"/>
-    </row>
-    <row r="31" spans="1:16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="29"/>
-      <c r="B31" s="40"/>
-      <c r="C31" s="27" t="s">
-        <v>716</v>
-      </c>
-      <c r="D31" s="27"/>
-      <c r="E31" s="33" t="s">
-        <v>156</v>
-      </c>
-      <c r="J31" s="27"/>
-      <c r="K31" s="27"/>
-      <c r="L31" s="27"/>
-      <c r="M31" s="27"/>
-      <c r="N31" s="27"/>
-      <c r="O31" s="27"/>
-      <c r="P31" s="27"/>
-    </row>
-    <row r="32" spans="1:16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="29"/>
-      <c r="B32" s="40"/>
-      <c r="C32" s="27" t="s">
-        <v>717</v>
-      </c>
-      <c r="D32" s="27"/>
-      <c r="E32" s="33" t="s">
-        <v>362</v>
-      </c>
-      <c r="J32" s="27"/>
-      <c r="K32" s="27"/>
-      <c r="L32" s="27"/>
-      <c r="M32" s="27"/>
-      <c r="N32" s="27"/>
-      <c r="O32" s="27"/>
-      <c r="P32" s="27"/>
-    </row>
+      <c r="M12" s="29"/>
+      <c r="N12" s="29"/>
+      <c r="O12" s="27"/>
+      <c r="P12" s="29"/>
+    </row>
+    <row r="13" spans="1:16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="14" spans="1:16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="1:16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="16" spans="1:16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="17" spans="1:16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="18" spans="1:16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="19" spans="1:16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="20" spans="1:16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="21" spans="1:16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="22" spans="1:16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="23" spans="1:16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="1:16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="1:16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="33" spans="1:16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="34" spans="1:16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="35" spans="1:16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="36" spans="1:16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="P4" r:id="rId1"/>
-    <hyperlink ref="P3" r:id="rId2"/>
+    <hyperlink ref="P2" r:id="rId1"/>
+    <hyperlink ref="P4" r:id="rId2"/>
     <hyperlink ref="P8" r:id="rId3"/>
-    <hyperlink ref="P2" r:id="rId4"/>
-    <hyperlink ref="P11" r:id="rId5"/>
-    <hyperlink ref="P16" r:id="rId6"/>
-    <hyperlink ref="P18" r:id="rId7"/>
-    <hyperlink ref="P21" r:id="rId8"/>
-    <hyperlink ref="P25" r:id="rId9"/>
-    <hyperlink ref="P29" r:id="rId10"/>
+    <hyperlink ref="P11" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId11"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C19:R30"/>
+  <sheetViews>
+    <sheetView topLeftCell="E14" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22:R30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="19" spans="3:18" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="C19" s="17" t="s">
+        <v>654</v>
+      </c>
+      <c r="D19" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="E19" s="19" t="s">
+        <v>655</v>
+      </c>
+      <c r="F19" s="20" t="s">
+        <v>465</v>
+      </c>
+      <c r="G19" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="H19" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="I19" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="J19" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="K19" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="L19" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="M19" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="N19" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="O19" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="P19" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q19" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="R19" s="37" t="s">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="20" spans="3:18" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="C20" s="22">
+        <v>308</v>
+      </c>
+      <c r="D20" s="23">
+        <v>42657</v>
+      </c>
+      <c r="E20" s="24" t="s">
+        <v>676</v>
+      </c>
+      <c r="F20" s="24" t="s">
+        <v>677</v>
+      </c>
+      <c r="G20" s="25" t="s">
+        <v>659</v>
+      </c>
+      <c r="H20" s="26"/>
+      <c r="I20" s="27">
+        <v>1112</v>
+      </c>
+      <c r="J20" s="27">
+        <v>150</v>
+      </c>
+      <c r="K20" s="27" t="s">
+        <v>646</v>
+      </c>
+      <c r="L20" s="27" t="s">
+        <v>178</v>
+      </c>
+      <c r="M20" s="27" t="s">
+        <v>658</v>
+      </c>
+      <c r="N20" s="28">
+        <v>6025002960</v>
+      </c>
+      <c r="O20" s="28"/>
+      <c r="P20" s="27"/>
+      <c r="Q20" s="27"/>
+      <c r="R20" s="36" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="21" spans="3:18" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="C21" s="29"/>
+      <c r="D21" s="30"/>
+      <c r="E21" s="31" t="s">
+        <v>657</v>
+      </c>
+      <c r="F21" s="32"/>
+      <c r="G21" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="H21" s="33"/>
+      <c r="I21" s="27"/>
+      <c r="J21" s="27"/>
+      <c r="K21" s="27"/>
+      <c r="L21" s="27"/>
+      <c r="M21" s="27"/>
+      <c r="N21" s="28"/>
+      <c r="O21" s="28"/>
+      <c r="P21" s="27"/>
+      <c r="Q21" s="27"/>
+      <c r="R21" s="36"/>
+    </row>
+    <row r="22" spans="3:18" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="C22" s="22">
+        <v>135</v>
+      </c>
+      <c r="D22" s="23">
+        <v>42658</v>
+      </c>
+      <c r="E22" s="24" t="s">
+        <v>673</v>
+      </c>
+      <c r="F22" s="25" t="s">
+        <v>661</v>
+      </c>
+      <c r="G22" s="24" t="s">
+        <v>662</v>
+      </c>
+      <c r="H22" s="26"/>
+      <c r="I22" s="27">
+        <v>1113</v>
+      </c>
+      <c r="J22" s="27">
+        <v>1001</v>
+      </c>
+      <c r="K22" s="27" t="s">
+        <v>647</v>
+      </c>
+      <c r="L22" s="27" t="s">
+        <v>134</v>
+      </c>
+      <c r="M22" s="27" t="s">
+        <v>135</v>
+      </c>
+      <c r="N22" s="28"/>
+      <c r="O22" s="28"/>
+      <c r="P22" s="27"/>
+      <c r="Q22" s="36" t="s">
+        <v>660</v>
+      </c>
+      <c r="R22" s="36"/>
+    </row>
+    <row r="23" spans="3:18" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="C23" s="29"/>
+      <c r="D23" s="30"/>
+      <c r="E23" s="31" t="s">
+        <v>674</v>
+      </c>
+      <c r="F23" s="27"/>
+      <c r="G23" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="H23" s="33"/>
+      <c r="I23" s="27"/>
+      <c r="J23" s="27"/>
+      <c r="K23" s="27"/>
+      <c r="L23" s="27"/>
+      <c r="M23" s="27"/>
+      <c r="N23" s="28"/>
+      <c r="O23" s="28"/>
+      <c r="P23" s="27"/>
+      <c r="Q23" s="36"/>
+      <c r="R23" s="36"/>
+    </row>
+    <row r="24" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="C24" s="29"/>
+      <c r="D24" s="30"/>
+      <c r="E24" s="31" t="s">
+        <v>663</v>
+      </c>
+      <c r="F24" s="27"/>
+      <c r="G24" s="32" t="s">
+        <v>156</v>
+      </c>
+      <c r="H24" s="33"/>
+      <c r="I24" s="27"/>
+      <c r="J24" s="27"/>
+      <c r="K24" s="27"/>
+      <c r="L24" s="27"/>
+      <c r="M24" s="27"/>
+      <c r="N24" s="28"/>
+      <c r="O24" s="28"/>
+      <c r="P24" s="27"/>
+      <c r="Q24" s="36"/>
+      <c r="R24" s="36"/>
+    </row>
+    <row r="25" spans="3:18" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="C25" s="29"/>
+      <c r="D25" s="30"/>
+      <c r="E25" s="31" t="s">
+        <v>664</v>
+      </c>
+      <c r="F25" s="27"/>
+      <c r="G25" s="32" t="s">
+        <v>665</v>
+      </c>
+      <c r="H25" s="33"/>
+      <c r="I25" s="27"/>
+      <c r="J25" s="27"/>
+      <c r="K25" s="27"/>
+      <c r="L25" s="27"/>
+      <c r="M25" s="27"/>
+      <c r="N25" s="28"/>
+      <c r="O25" s="28"/>
+      <c r="P25" s="27"/>
+      <c r="Q25" s="36"/>
+      <c r="R25" s="36"/>
+    </row>
+    <row r="26" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="C26" s="38">
+        <v>193</v>
+      </c>
+      <c r="D26" s="23">
+        <v>42910</v>
+      </c>
+      <c r="E26" s="25" t="s">
+        <v>672</v>
+      </c>
+      <c r="F26" s="25" t="s">
+        <v>666</v>
+      </c>
+      <c r="G26" s="25" t="s">
+        <v>667</v>
+      </c>
+      <c r="H26" s="25"/>
+      <c r="L26" s="27" t="s">
+        <v>151</v>
+      </c>
+      <c r="M26" s="27" t="s">
+        <v>670</v>
+      </c>
+      <c r="N26" s="28" t="s">
+        <v>671</v>
+      </c>
+      <c r="O26" s="28"/>
+      <c r="P26" s="28"/>
+      <c r="Q26" s="41" t="s">
+        <v>683</v>
+      </c>
+      <c r="R26" s="41"/>
+    </row>
+    <row r="27" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="C27" s="29"/>
+      <c r="D27" s="30"/>
+      <c r="E27" s="27" t="s">
+        <v>675</v>
+      </c>
+      <c r="F27" s="27"/>
+      <c r="G27" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="H27" s="33"/>
+      <c r="L27" s="27"/>
+      <c r="M27" s="27"/>
+      <c r="N27" s="28"/>
+      <c r="O27" s="28"/>
+      <c r="P27" s="28"/>
+      <c r="Q27" s="28"/>
+      <c r="R27" s="28"/>
+    </row>
+    <row r="28" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="C28" s="29"/>
+      <c r="D28" s="30"/>
+      <c r="E28" s="27" t="s">
+        <v>668</v>
+      </c>
+      <c r="F28" s="27"/>
+      <c r="G28" s="33" t="s">
+        <v>36</v>
+      </c>
+      <c r="H28" s="33" t="s">
+        <v>669</v>
+      </c>
+      <c r="L28" s="27"/>
+      <c r="M28" s="27"/>
+      <c r="N28" s="28"/>
+      <c r="O28" s="28"/>
+      <c r="P28" s="28"/>
+      <c r="Q28" s="28"/>
+      <c r="R28" s="28"/>
+    </row>
+    <row r="29" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="C29" s="38">
+        <v>238</v>
+      </c>
+      <c r="D29" s="39">
+        <v>42987</v>
+      </c>
+      <c r="E29" s="25" t="s">
+        <v>682</v>
+      </c>
+      <c r="F29" s="25" t="s">
+        <v>678</v>
+      </c>
+      <c r="G29" s="25" t="s">
+        <v>104</v>
+      </c>
+      <c r="H29" s="25" t="s">
+        <v>112</v>
+      </c>
+      <c r="L29" s="27" t="s">
+        <v>178</v>
+      </c>
+      <c r="M29" s="27" t="s">
+        <v>658</v>
+      </c>
+      <c r="N29" s="27" t="s">
+        <v>680</v>
+      </c>
+      <c r="O29" s="28" t="s">
+        <v>681</v>
+      </c>
+      <c r="P29" s="28"/>
+      <c r="Q29" s="41" t="s">
+        <v>684</v>
+      </c>
+      <c r="R29" s="41"/>
+    </row>
+    <row r="30" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="C30" s="29"/>
+      <c r="D30" s="40"/>
+      <c r="E30" s="27" t="s">
+        <v>679</v>
+      </c>
+      <c r="F30" s="27"/>
+      <c r="G30" s="33" t="s">
+        <v>156</v>
+      </c>
+      <c r="H30" s="33" t="s">
+        <v>37</v>
+      </c>
+      <c r="L30" s="27"/>
+      <c r="M30" s="27"/>
+      <c r="N30" s="27"/>
+      <c r="O30" s="29"/>
+      <c r="P30" s="29"/>
+      <c r="Q30" s="29"/>
+      <c r="R30" s="29"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="R20" r:id="rId1"/>
+    <hyperlink ref="Q22" r:id="rId2"/>
+    <hyperlink ref="Q26" r:id="rId3"/>
+    <hyperlink ref="Q29" r:id="rId4"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X210"/>
   <sheetViews>
@@ -7952,7 +7985,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E171"/>
   <sheetViews>
@@ -10621,7 +10654,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I22"/>
   <sheetViews>

</xml_diff>